<commit_message>
Modificaciones a escaleta 11_13
Modificaciones a escaleta 11_13
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion13/ESCALETA FINAL CN_11_13_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion13/ESCALETA FINAL CN_11_13_CO.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="20490" windowHeight="7695"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="DATOS" sheetId="2" r:id="rId2"/>
+    <sheet name="DATOS" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$U$39</definedName>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="217">
   <si>
     <t>Asignatura</t>
   </si>
@@ -450,15 +455,9 @@
     <t>Interactivo que permite presentar generalidades de los compuestos orgánicos nitrogenados</t>
   </si>
   <si>
-    <t>Diaporama F1-03</t>
-  </si>
-  <si>
     <t>Los alcaloides</t>
   </si>
   <si>
-    <t>Recurso F6-04</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: Los ésteres</t>
   </si>
   <si>
@@ -660,13 +659,34 @@
     <t>Diaporama F1-02</t>
   </si>
   <si>
-    <t>Diaporama F1-04</t>
-  </si>
-  <si>
-    <t>Diaporama F1-05</t>
-  </si>
-  <si>
-    <t>Diaporama F1-06</t>
+    <t>Recurso FQ_10_13_08-01</t>
+  </si>
+  <si>
+    <t>Recurso FQ_10_13_08-02</t>
+  </si>
+  <si>
+    <t>Recurso FQ_10_13_08-03</t>
+  </si>
+  <si>
+    <t>Recurso F6-02</t>
+  </si>
+  <si>
+    <t>Recurso F6-03</t>
+  </si>
+  <si>
+    <t>Recurso FQ_10_13_08-04</t>
+  </si>
+  <si>
+    <t>Recurso FQ_10_13_08-05</t>
+  </si>
+  <si>
+    <t>Recurso F7-01</t>
+  </si>
+  <si>
+    <t>SECUENCIA DE IMAG</t>
+  </si>
+  <si>
+    <t>FQ</t>
   </si>
 </sst>
 </file>
@@ -702,7 +722,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -748,6 +768,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1001,7 +1033,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1083,6 +1115,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1374,7 +1415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1384,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K39" sqref="A39:XFD39"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1413,94 +1454,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="52" t="s">
+      <c r="L1" s="55" t="s">
         <v>10</v>
       </c>
       <c r="M1" s="49"/>
       <c r="N1" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="50" t="s">
+      <c r="O1" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="50" t="s">
+      <c r="P1" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="50" t="s">
+      <c r="Q1" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="50" t="s">
+      <c r="R1" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="50" t="s">
+      <c r="S1" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="50" t="s">
+      <c r="T1" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="50" t="s">
+      <c r="U1" s="53" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="10" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="53"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="56"/>
       <c r="M2" s="48" t="s">
         <v>87</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -1577,16 +1618,16 @@
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="H4" s="30">
+        <v>192</v>
+      </c>
+      <c r="H4" s="50">
         <v>2</v>
       </c>
       <c r="I4" s="30" t="s">
         <v>20</v>
       </c>
       <c r="J4" s="31" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K4" s="36" t="s">
         <v>69</v>
@@ -1594,10 +1635,10 @@
       <c r="L4" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42" t="s">
+        <v>216</v>
+      </c>
       <c r="O4" s="42"/>
       <c r="P4" s="40" t="s">
         <v>19</v>
@@ -1612,7 +1653,7 @@
         <v>132</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>133</v>
+        <v>207</v>
       </c>
       <c r="U4" s="2" t="s">
         <v>134</v>
@@ -1636,7 +1677,7 @@
       </c>
       <c r="F5" s="24"/>
       <c r="G5" s="29" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H5" s="30">
         <v>3</v>
@@ -1645,7 +1686,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K5" s="36" t="s">
         <v>69</v>
@@ -1668,13 +1709,13 @@
         <v>131</v>
       </c>
       <c r="S5" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="U5" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T5" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1728,7 +1769,7 @@
       </c>
       <c r="F7" s="26"/>
       <c r="G7" s="32" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H7" s="33">
         <v>4</v>
@@ -1737,7 +1778,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="34" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="K7" s="38" t="s">
         <v>69</v>
@@ -1760,13 +1801,13 @@
         <v>131</v>
       </c>
       <c r="S7" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="U7" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T7" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -1787,7 +1828,7 @@
       </c>
       <c r="F8" s="26"/>
       <c r="G8" s="32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H8" s="33">
         <v>5</v>
@@ -1796,7 +1837,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="34" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K8" s="38" t="s">
         <v>69</v>
@@ -1809,7 +1850,9 @@
         <v>62</v>
       </c>
       <c r="O8" s="41"/>
-      <c r="P8" s="40"/>
+      <c r="P8" s="40" t="s">
+        <v>19</v>
+      </c>
       <c r="Q8" s="1">
         <v>6</v>
       </c>
@@ -1817,13 +1860,13 @@
         <v>131</v>
       </c>
       <c r="S8" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T8" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="U8" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T8" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -1844,16 +1887,16 @@
       </c>
       <c r="F9" s="26"/>
       <c r="G9" s="32" t="s">
-        <v>196</v>
-      </c>
-      <c r="H9" s="33">
+        <v>194</v>
+      </c>
+      <c r="H9" s="51">
         <v>6</v>
       </c>
       <c r="I9" s="33" t="s">
         <v>20</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K9" s="38" t="s">
         <v>69</v>
@@ -1861,12 +1904,14 @@
       <c r="L9" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42" t="s">
+        <v>216</v>
+      </c>
       <c r="O9" s="41"/>
-      <c r="P9" s="40"/>
+      <c r="P9" s="40" t="s">
+        <v>19</v>
+      </c>
       <c r="Q9" s="1">
         <v>6</v>
       </c>
@@ -1936,7 +1981,7 @@
       <c r="G11" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="H11" s="33">
+      <c r="H11" s="52">
         <v>7</v>
       </c>
       <c r="I11" s="33" t="s">
@@ -1948,7 +1993,9 @@
       <c r="K11" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="L11" s="39"/>
+      <c r="L11" s="39" t="s">
+        <v>215</v>
+      </c>
       <c r="M11" s="42" t="s">
         <v>34</v>
       </c>
@@ -1967,7 +2014,7 @@
         <v>132</v>
       </c>
       <c r="T11" s="11" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>134</v>
@@ -1991,7 +2038,7 @@
       </c>
       <c r="F12" s="26"/>
       <c r="G12" s="32" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H12" s="33">
         <v>8</v>
@@ -2000,7 +2047,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="34" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K12" s="38" t="s">
         <v>69</v>
@@ -2013,7 +2060,9 @@
         <v>62</v>
       </c>
       <c r="O12" s="41"/>
-      <c r="P12" s="40"/>
+      <c r="P12" s="40" t="s">
+        <v>19</v>
+      </c>
       <c r="Q12" s="1">
         <v>6</v>
       </c>
@@ -2021,13 +2070,13 @@
         <v>131</v>
       </c>
       <c r="S12" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T12" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="U12" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T12" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2081,7 +2130,7 @@
       </c>
       <c r="F14" s="26"/>
       <c r="G14" s="32" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H14" s="33">
         <v>9</v>
@@ -2090,7 +2139,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="34" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K14" s="38" t="s">
         <v>69</v>
@@ -2113,13 +2162,13 @@
         <v>131</v>
       </c>
       <c r="S14" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T14" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="U14" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T14" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2140,7 +2189,7 @@
       </c>
       <c r="F15" s="26"/>
       <c r="G15" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H15" s="33">
         <v>10</v>
@@ -2149,7 +2198,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="34" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K15" s="38" t="s">
         <v>69</v>
@@ -2172,13 +2221,13 @@
         <v>131</v>
       </c>
       <c r="S15" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T15" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="U15" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T15" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2199,7 +2248,7 @@
       </c>
       <c r="F16" s="26"/>
       <c r="G16" s="32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H16" s="33">
         <v>11</v>
@@ -2208,7 +2257,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="34" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K16" s="38" t="s">
         <v>69</v>
@@ -2231,13 +2280,13 @@
         <v>131</v>
       </c>
       <c r="S16" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T16" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="U16" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T16" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -2293,7 +2342,7 @@
       <c r="G18" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="H18" s="33">
+      <c r="H18" s="52">
         <v>12</v>
       </c>
       <c r="I18" s="33" t="s">
@@ -2326,7 +2375,7 @@
         <v>127</v>
       </c>
       <c r="T18" s="11" t="s">
-        <v>128</v>
+        <v>210</v>
       </c>
       <c r="U18" s="2" t="s">
         <v>129</v>
@@ -2350,7 +2399,7 @@
       </c>
       <c r="F19" s="26"/>
       <c r="G19" s="32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H19" s="33">
         <v>13</v>
@@ -2359,7 +2408,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K19" s="38" t="s">
         <v>69</v>
@@ -2372,7 +2421,9 @@
         <v>62</v>
       </c>
       <c r="O19" s="41"/>
-      <c r="P19" s="40"/>
+      <c r="P19" s="40" t="s">
+        <v>19</v>
+      </c>
       <c r="Q19" s="1">
         <v>6</v>
       </c>
@@ -2380,13 +2431,13 @@
         <v>131</v>
       </c>
       <c r="S19" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T19" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="U19" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T19" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="U19" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -2407,30 +2458,46 @@
       </c>
       <c r="F20" s="26"/>
       <c r="G20" s="32" t="s">
-        <v>193</v>
-      </c>
-      <c r="H20" s="33">
+        <v>191</v>
+      </c>
+      <c r="H20" s="51">
         <v>14</v>
       </c>
       <c r="I20" s="33" t="s">
         <v>20</v>
       </c>
       <c r="J20" s="31" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K20" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="L20" s="39"/>
+      <c r="L20" s="39" t="s">
+        <v>32</v>
+      </c>
       <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
+      <c r="N20" s="42" t="s">
+        <v>216</v>
+      </c>
       <c r="O20" s="41"/>
-      <c r="P20" s="40"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
-      <c r="U20" s="2"/>
+      <c r="P20" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>6</v>
+      </c>
+      <c r="R20" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="S20" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="T20" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="U20" s="2" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
@@ -2485,7 +2552,7 @@
       <c r="G22" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="H22" s="33">
+      <c r="H22" s="52">
         <v>15</v>
       </c>
       <c r="I22" s="33" t="s">
@@ -2497,7 +2564,9 @@
       <c r="K22" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="L22" s="39"/>
+      <c r="L22" s="39" t="s">
+        <v>215</v>
+      </c>
       <c r="M22" s="42" t="s">
         <v>34</v>
       </c>
@@ -2516,7 +2585,7 @@
         <v>132</v>
       </c>
       <c r="T22" s="11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="U22" s="2" t="s">
         <v>134</v>
@@ -2540,7 +2609,7 @@
       </c>
       <c r="F23" s="26"/>
       <c r="G23" s="32" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H23" s="33">
         <v>16</v>
@@ -2549,7 +2618,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K23" s="38" t="s">
         <v>69</v>
@@ -2562,7 +2631,9 @@
         <v>62</v>
       </c>
       <c r="O23" s="41"/>
-      <c r="P23" s="40"/>
+      <c r="P23" s="40" t="s">
+        <v>19</v>
+      </c>
       <c r="Q23" s="1">
         <v>6</v>
       </c>
@@ -2570,13 +2641,13 @@
         <v>131</v>
       </c>
       <c r="S23" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="U23" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="U23" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -2634,16 +2705,16 @@
         <v>114</v>
       </c>
       <c r="G25" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="H25" s="33">
+        <v>199</v>
+      </c>
+      <c r="H25" s="51">
         <v>17</v>
       </c>
       <c r="I25" s="33" t="s">
         <v>20</v>
       </c>
       <c r="J25" s="31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K25" s="38" t="s">
         <v>69</v>
@@ -2651,10 +2722,10 @@
       <c r="L25" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="M25" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="N25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42" t="s">
+        <v>216</v>
+      </c>
       <c r="O25" s="41"/>
       <c r="P25" s="40" t="s">
         <v>19</v>
@@ -2669,7 +2740,7 @@
         <v>132</v>
       </c>
       <c r="T25" s="11" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="U25" s="2" t="s">
         <v>134</v>
@@ -2695,7 +2766,7 @@
         <v>114</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H26" s="33">
         <v>18</v>
@@ -2704,7 +2775,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="31" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K26" s="38" t="s">
         <v>69</v>
@@ -2727,13 +2798,13 @@
         <v>131</v>
       </c>
       <c r="S26" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T26" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="U26" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T26" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="U26" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -2791,16 +2862,16 @@
         <v>116</v>
       </c>
       <c r="G28" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="H28" s="33">
+        <v>139</v>
+      </c>
+      <c r="H28" s="52">
         <v>19</v>
       </c>
       <c r="I28" s="33" t="s">
         <v>19</v>
       </c>
       <c r="J28" s="34" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K28" s="38" t="s">
         <v>69</v>
@@ -2826,7 +2897,7 @@
         <v>127</v>
       </c>
       <c r="T28" s="11" t="s">
-        <v>141</v>
+        <v>211</v>
       </c>
       <c r="U28" s="2" t="s">
         <v>129</v>
@@ -2887,16 +2958,16 @@
         <v>119</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>202</v>
-      </c>
-      <c r="H30" s="33">
+        <v>200</v>
+      </c>
+      <c r="H30" s="51">
         <v>20</v>
       </c>
       <c r="I30" s="33" t="s">
         <v>20</v>
       </c>
       <c r="J30" s="31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K30" s="38" t="s">
         <v>69</v>
@@ -2904,10 +2975,10 @@
       <c r="L30" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="M30" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="N30" s="42"/>
+      <c r="M30" s="42"/>
+      <c r="N30" s="42" t="s">
+        <v>216</v>
+      </c>
       <c r="O30" s="41"/>
       <c r="P30" s="40" t="s">
         <v>19</v>
@@ -2922,7 +2993,7 @@
         <v>132</v>
       </c>
       <c r="T30" s="11" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="U30" s="2" t="s">
         <v>134</v>
@@ -2950,7 +3021,7 @@
       <c r="G31" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="H31" s="33">
+      <c r="H31" s="51">
         <v>21</v>
       </c>
       <c r="I31" s="33" t="s">
@@ -2966,7 +3037,7 @@
         <v>31</v>
       </c>
       <c r="M31" s="42" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="N31" s="42"/>
       <c r="O31" s="41"/>
@@ -2977,16 +3048,16 @@
         <v>6</v>
       </c>
       <c r="R31" s="11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="S31" s="11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="T31" s="11" t="s">
-        <v>139</v>
+        <v>214</v>
       </c>
       <c r="U31" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
@@ -3007,7 +3078,7 @@
       </c>
       <c r="F32" s="26"/>
       <c r="G32" s="32" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H32" s="33">
         <v>22</v>
@@ -3016,7 +3087,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K32" s="38" t="s">
         <v>69</v>
@@ -3039,13 +3110,13 @@
         <v>131</v>
       </c>
       <c r="S32" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T32" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="U32" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T32" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="U32" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3064,7 +3135,7 @@
       <c r="E33" s="25"/>
       <c r="F33" s="26"/>
       <c r="G33" s="47" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H33" s="33">
         <v>23</v>
@@ -3073,7 +3144,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="34" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K33" s="38" t="s">
         <v>69</v>
@@ -3096,13 +3167,13 @@
         <v>131</v>
       </c>
       <c r="S33" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T33" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="U33" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T33" s="11" t="s">
-        <v>163</v>
-      </c>
-      <c r="U33" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -3121,7 +3192,7 @@
       <c r="E34" s="25"/>
       <c r="F34" s="26"/>
       <c r="G34" s="32" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H34" s="33">
         <v>24</v>
@@ -3130,7 +3201,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K34" s="38" t="s">
         <v>69</v>
@@ -3153,13 +3224,13 @@
         <v>131</v>
       </c>
       <c r="S34" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T34" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="U34" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T34" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="U34" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3178,7 +3249,7 @@
       <c r="E35" s="25"/>
       <c r="F35" s="26"/>
       <c r="G35" s="47" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H35" s="33">
         <v>25</v>
@@ -3187,7 +3258,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K35" s="38" t="s">
         <v>69</v>
@@ -3210,13 +3281,13 @@
         <v>131</v>
       </c>
       <c r="S35" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T35" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="U35" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T35" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="U35" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3235,7 +3306,7 @@
       <c r="E36" s="25"/>
       <c r="F36" s="26"/>
       <c r="G36" s="47" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H36" s="33">
         <v>26</v>
@@ -3244,7 +3315,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K36" s="38" t="s">
         <v>69</v>
@@ -3267,13 +3338,13 @@
         <v>131</v>
       </c>
       <c r="S36" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T36" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="U36" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T36" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="U36" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -3292,14 +3363,14 @@
       <c r="E37" s="25"/>
       <c r="F37" s="26"/>
       <c r="G37" s="32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H37" s="33">
         <v>27</v>
       </c>
       <c r="I37" s="33"/>
       <c r="J37" s="34" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K37" s="38" t="s">
         <v>69</v>
@@ -3335,7 +3406,7 @@
       <c r="E38" s="25"/>
       <c r="F38" s="26"/>
       <c r="G38" s="32" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H38" s="33">
         <v>28</v>
@@ -3344,7 +3415,7 @@
         <v>20</v>
       </c>
       <c r="J38" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K38" s="38" t="s">
         <v>69</v>
@@ -3367,13 +3438,13 @@
         <v>131</v>
       </c>
       <c r="S38" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T38" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="U38" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T38" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="U38" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3390,7 +3461,7 @@
       <c r="E39" s="25"/>
       <c r="F39" s="26"/>
       <c r="G39" s="47" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H39" s="33">
         <v>29</v>
@@ -3399,7 +3470,7 @@
         <v>20</v>
       </c>
       <c r="J39" s="34" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K39" s="38" t="s">
         <v>69</v>
@@ -3422,13 +3493,13 @@
         <v>131</v>
       </c>
       <c r="S39" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="T39" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="U39" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="T39" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="U39" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
@@ -4766,6 +4837,7 @@
       <c r="U97" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:U39"/>
   <mergeCells count="19">
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>

</xml_diff>

<commit_message>
Cambio de lugar recursos 11_13
Cambio de lugar recursos 11_13
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion13/ESCALETA FINAL CN_11_13_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion13/ESCALETA FINAL CN_11_13_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="20490" windowHeight="7695"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="DATOS" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$U$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$U$42</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
@@ -23,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="219">
   <si>
     <t>Asignatura</t>
   </si>
@@ -405,12 +410,6 @@
     <t>Interactivo que permite presentar generalidades de los ésteres</t>
   </si>
   <si>
-    <t xml:space="preserve">Los ésteres </t>
-  </si>
-  <si>
-    <t>Los haluros de ácido</t>
-  </si>
-  <si>
     <t>RF</t>
   </si>
   <si>
@@ -423,9 +422,6 @@
     <t>RF_01_01_CO</t>
   </si>
   <si>
-    <t>Secuencia de imágenes que permite explicar los anhídridos de ácido</t>
-  </si>
-  <si>
     <t>RM</t>
   </si>
   <si>
@@ -444,12 +440,6 @@
     <t>Secuencia de imágenes que permiten exponer las generalidades de los haluros de ácido</t>
   </si>
   <si>
-    <t xml:space="preserve">Las funciones nitrogenadas </t>
-  </si>
-  <si>
-    <t>Interactivo que permite presentar generalidades de los compuestos orgánicos nitrogenados</t>
-  </si>
-  <si>
     <t>Los alcaloides</t>
   </si>
   <si>
@@ -682,6 +672,27 @@
   </si>
   <si>
     <t>FQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La función éster </t>
+  </si>
+  <si>
+    <t>La función amida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los anhídridos carboxílicos </t>
+  </si>
+  <si>
+    <t>Secuencia de imágenes que permite explicar los anhídridos de ácidos carboxílicos</t>
+  </si>
+  <si>
+    <t>Las características de los haluros de ácido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los compuestos nitrogenados </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interactivo que permite presentar generalidades de las aminas y nitrilos </t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1039,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1111,13 +1122,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1137,6 +1142,39 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1410,7 +1448,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1418,10 +1456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U97"/>
+  <dimension ref="A1:U100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,94 +1487,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="53" t="s">
         <v>10</v>
       </c>
       <c r="M1" s="49"/>
       <c r="N1" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="53" t="s">
+      <c r="O1" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="53" t="s">
+      <c r="P1" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="53" t="s">
+      <c r="Q1" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="53" t="s">
+      <c r="R1" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="53" t="s">
+      <c r="S1" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="53" t="s">
+      <c r="T1" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="53" t="s">
+      <c r="U1" s="51" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="10" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="56"/>
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="54"/>
       <c r="M2" s="48" t="s">
         <v>87</v>
       </c>
       <c r="N2" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="52"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="52"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -1554,9 +1592,9 @@
       <c r="E3" s="24"/>
       <c r="F3" s="24"/>
       <c r="G3" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="H3" s="30">
+        <v>212</v>
+      </c>
+      <c r="H3" s="33">
         <v>1</v>
       </c>
       <c r="I3" s="30" t="s">
@@ -1583,16 +1621,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="T3" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="U3" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="T3" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1613,16 +1651,16 @@
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="H4" s="50">
+        <v>187</v>
+      </c>
+      <c r="H4" s="33">
         <v>2</v>
       </c>
       <c r="I4" s="30" t="s">
         <v>20</v>
       </c>
       <c r="J4" s="31" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="K4" s="36" t="s">
         <v>69</v>
@@ -1632,7 +1670,7 @@
       </c>
       <c r="M4" s="42"/>
       <c r="N4" s="42" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="O4" s="42"/>
       <c r="P4" s="40" t="s">
@@ -1642,16 +1680,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="U4" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="T4" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1672,16 +1710,16 @@
       </c>
       <c r="F5" s="24"/>
       <c r="G5" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="H5" s="30">
+        <v>185</v>
+      </c>
+      <c r="H5" s="33">
         <v>3</v>
       </c>
       <c r="I5" s="30" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="K5" s="36" t="s">
         <v>69</v>
@@ -1701,16 +1739,16 @@
         <v>6</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="S5" s="11" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="T5" s="11" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1764,7 +1802,7 @@
       </c>
       <c r="F7" s="26"/>
       <c r="G7" s="32" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H7" s="33">
         <v>4</v>
@@ -1773,7 +1811,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="34" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="K7" s="38" t="s">
         <v>69</v>
@@ -1793,16 +1831,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="T7" s="11" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -1823,7 +1861,7 @@
       </c>
       <c r="F8" s="26"/>
       <c r="G8" s="32" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H8" s="33">
         <v>5</v>
@@ -1832,7 +1870,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="34" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="K8" s="38" t="s">
         <v>69</v>
@@ -1852,75 +1890,73 @@
         <v>6</v>
       </c>
       <c r="R8" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="T8" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="61"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="60" t="s">
+        <v>214</v>
+      </c>
+      <c r="H9" s="50">
+        <v>6</v>
+      </c>
+      <c r="I9" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="63" t="s">
+        <v>215</v>
+      </c>
+      <c r="K9" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="L9" s="64" t="s">
+        <v>210</v>
+      </c>
+      <c r="M9" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" s="65"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="68">
+        <v>6</v>
+      </c>
+      <c r="R9" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="S9" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="T9" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="U9" s="70" t="s">
         <v>131</v>
-      </c>
-      <c r="S8" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="T8" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="32" t="s">
-        <v>194</v>
-      </c>
-      <c r="H9" s="51">
-        <v>6</v>
-      </c>
-      <c r="I9" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="31" t="s">
-        <v>195</v>
-      </c>
-      <c r="K9" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="L9" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="M9" s="42"/>
-      <c r="N9" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="O9" s="41"/>
-      <c r="P9" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>6</v>
-      </c>
-      <c r="R9" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="S9" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="T9" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -1937,24 +1973,50 @@
         <v>97</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F10" s="26"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="39"/>
+      <c r="G10" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="H10" s="33">
+        <v>7</v>
+      </c>
+      <c r="I10" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="K10" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="39" t="s">
+        <v>32</v>
+      </c>
       <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
+      <c r="N10" s="42" t="s">
+        <v>211</v>
+      </c>
       <c r="O10" s="41"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="2"/>
+      <c r="P10" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>6</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="T10" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
@@ -1969,51 +2031,25 @@
       <c r="D11" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="H11" s="52">
-        <v>7</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="34" t="s">
-        <v>130</v>
-      </c>
-      <c r="K11" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="L11" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="M11" s="42" t="s">
-        <v>34</v>
-      </c>
+      <c r="E11" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" s="26"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="42"/>
       <c r="N11" s="42"/>
       <c r="O11" s="41"/>
-      <c r="P11" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>6</v>
-      </c>
-      <c r="R11" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="S11" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="T11" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="U11" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="2"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -2028,53 +2064,27 @@
       <c r="D12" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="H12" s="33">
-        <v>8</v>
-      </c>
-      <c r="I12" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="K12" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="L12" s="39" t="s">
-        <v>32</v>
-      </c>
+      <c r="E12" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" s="24"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="39"/>
       <c r="M12" s="42"/>
-      <c r="N12" s="42" t="s">
-        <v>62</v>
-      </c>
+      <c r="N12" s="42"/>
       <c r="O12" s="41"/>
-      <c r="P12" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>6</v>
-      </c>
-      <c r="R12" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="S12" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="T12" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="40"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>67</v>
       </c>
@@ -2085,85 +2095,109 @@
         <v>91</v>
       </c>
       <c r="D13" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="26"/>
+      <c r="G13" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="H13" s="33">
+        <v>8</v>
+      </c>
+      <c r="I13" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="K13" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="M13" s="42"/>
+      <c r="N13" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="O13" s="41"/>
+      <c r="P13" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>6</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="S13" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="T13" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="40"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="2"/>
-    </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="E14" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="32" t="s">
-        <v>196</v>
-      </c>
-      <c r="H14" s="33">
+      <c r="E14" s="61"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="60" t="s">
+        <v>213</v>
+      </c>
+      <c r="H14" s="50">
         <v>9</v>
       </c>
-      <c r="I14" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="34" t="s">
-        <v>197</v>
-      </c>
-      <c r="K14" s="38" t="s">
+      <c r="I14" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="63" t="s">
+        <v>132</v>
+      </c>
+      <c r="K14" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="L14" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="O14" s="41"/>
-      <c r="P14" s="40" t="s">
+      <c r="L14" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="N14" s="65"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="Q14" s="68">
         <v>6</v>
       </c>
-      <c r="R14" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="S14" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="T14" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>154</v>
+      <c r="R14" s="69" t="s">
+        <v>124</v>
+      </c>
+      <c r="S14" s="69" t="s">
+        <v>125</v>
+      </c>
+      <c r="T14" s="69" t="s">
+        <v>205</v>
+      </c>
+      <c r="U14" s="70" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2180,50 +2214,24 @@
         <v>101</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F15" s="26"/>
-      <c r="G15" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="H15" s="33">
-        <v>10</v>
-      </c>
-      <c r="I15" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="K15" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="L15" s="39" t="s">
-        <v>32</v>
-      </c>
+      <c r="G15" s="32"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="39"/>
       <c r="M15" s="42"/>
-      <c r="N15" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="O15" s="42"/>
-      <c r="P15" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>6</v>
-      </c>
-      <c r="R15" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="S15" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="T15" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="N15" s="42"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="2"/>
     </row>
     <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
@@ -2243,16 +2251,16 @@
       </c>
       <c r="F16" s="26"/>
       <c r="G16" s="32" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="H16" s="33">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I16" s="33" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="34" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="K16" s="38" t="s">
         <v>69</v>
@@ -2262,9 +2270,9 @@
       </c>
       <c r="M16" s="42"/>
       <c r="N16" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="O16" s="42"/>
+        <v>81</v>
+      </c>
+      <c r="O16" s="41"/>
       <c r="P16" s="40" t="s">
         <v>19</v>
       </c>
@@ -2272,19 +2280,19 @@
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="S16" s="11" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="T16" s="11" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>67</v>
       </c>
@@ -2298,26 +2306,52 @@
         <v>101</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F17" s="26"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="38"/>
-      <c r="L17" s="39"/>
+      <c r="G17" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="H17" s="33">
+        <v>11</v>
+      </c>
+      <c r="I17" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="K17" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="L17" s="39" t="s">
+        <v>32</v>
+      </c>
       <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="41"/>
-      <c r="P17" s="40"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="2"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N17" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="O17" s="42"/>
+      <c r="P17" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>6</v>
+      </c>
+      <c r="R17" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="S17" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="T17" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>67</v>
       </c>
@@ -2331,32 +2365,32 @@
         <v>101</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F18" s="26"/>
       <c r="G18" s="32" t="s">
-        <v>101</v>
-      </c>
-      <c r="H18" s="52">
+        <v>160</v>
+      </c>
+      <c r="H18" s="33">
         <v>12</v>
       </c>
       <c r="I18" s="33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J18" s="34" t="s">
-        <v>135</v>
+        <v>181</v>
       </c>
       <c r="K18" s="38" t="s">
         <v>69</v>
       </c>
       <c r="L18" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="M18" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="N18" s="42"/>
-      <c r="O18" s="41"/>
+        <v>32</v>
+      </c>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="O18" s="42"/>
       <c r="P18" s="40" t="s">
         <v>19</v>
       </c>
@@ -2364,16 +2398,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="S18" s="11" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="T18" s="11" t="s">
-        <v>210</v>
+        <v>161</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -2389,51 +2423,25 @@
       <c r="D19" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="45" t="s">
-        <v>106</v>
+      <c r="E19" s="25" t="s">
+        <v>104</v>
       </c>
       <c r="F19" s="26"/>
-      <c r="G19" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="H19" s="33">
-        <v>13</v>
-      </c>
-      <c r="I19" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J19" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="K19" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="L19" s="39" t="s">
-        <v>32</v>
-      </c>
+      <c r="G19" s="32"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="39"/>
       <c r="M19" s="42"/>
-      <c r="N19" s="42" t="s">
-        <v>62</v>
-      </c>
+      <c r="N19" s="42"/>
       <c r="O19" s="41"/>
-      <c r="P19" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q19" s="1">
-        <v>6</v>
-      </c>
-      <c r="R19" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="S19" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="T19" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="U19" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="2"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
@@ -2445,54 +2453,28 @@
       <c r="C20" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="46" t="s">
-        <v>107</v>
+      <c r="D20" s="21" t="s">
+        <v>101</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F20" s="26"/>
-      <c r="G20" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="H20" s="51">
-        <v>14</v>
-      </c>
-      <c r="I20" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J20" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="K20" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="L20" s="39" t="s">
-        <v>32</v>
-      </c>
+      <c r="G20" s="32"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="39"/>
       <c r="M20" s="42"/>
-      <c r="N20" s="42" t="s">
-        <v>216</v>
-      </c>
+      <c r="N20" s="42"/>
       <c r="O20" s="41"/>
-      <c r="P20" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>6</v>
-      </c>
-      <c r="R20" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="S20" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="T20" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="U20" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="2"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
@@ -2504,86 +2486,110 @@
       <c r="C21" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="F21" s="26"/>
+      <c r="G21" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" s="33">
+        <v>13</v>
+      </c>
+      <c r="I21" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="K21" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="M21" s="42"/>
+      <c r="N21" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="O21" s="41"/>
+      <c r="P21" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>6</v>
+      </c>
+      <c r="R21" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="S21" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="T21" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="58" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="71" t="s">
         <v>107</v>
       </c>
-      <c r="E21" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="38"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="41"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="2"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" s="46" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" s="26"/>
-      <c r="G22" s="32" t="s">
-        <v>125</v>
-      </c>
-      <c r="H22" s="52">
-        <v>15</v>
-      </c>
-      <c r="I22" s="33" t="s">
+      <c r="E22" s="61"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="60" t="s">
+        <v>216</v>
+      </c>
+      <c r="H22" s="50">
+        <v>14</v>
+      </c>
+      <c r="I22" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="J22" s="34" t="s">
-        <v>136</v>
-      </c>
-      <c r="K22" s="38" t="s">
+      <c r="J22" s="63" t="s">
+        <v>133</v>
+      </c>
+      <c r="K22" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="L22" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="M22" s="42" t="s">
+      <c r="L22" s="64" t="s">
+        <v>210</v>
+      </c>
+      <c r="M22" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="N22" s="42"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="40" t="s">
+      <c r="N22" s="65"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="1">
+      <c r="Q22" s="68">
         <v>6</v>
       </c>
-      <c r="R22" s="11" t="s">
+      <c r="R22" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="S22" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="T22" s="69" t="s">
+        <v>201</v>
+      </c>
+      <c r="U22" s="70" t="s">
         <v>131</v>
-      </c>
-      <c r="S22" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="T22" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -2600,20 +2606,20 @@
         <v>107</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="F23" s="26"/>
       <c r="G23" s="32" t="s">
-        <v>146</v>
+        <v>186</v>
       </c>
       <c r="H23" s="33">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I23" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="34" t="s">
-        <v>148</v>
+      <c r="J23" s="31" t="s">
+        <v>165</v>
       </c>
       <c r="K23" s="38" t="s">
         <v>69</v>
@@ -2623,7 +2629,7 @@
       </c>
       <c r="M23" s="42"/>
       <c r="N23" s="42" t="s">
-        <v>62</v>
+        <v>211</v>
       </c>
       <c r="O23" s="41"/>
       <c r="P23" s="40" t="s">
@@ -2633,16 +2639,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="S23" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="U23" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="S23" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="T23" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="U23" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -2655,19 +2661,17 @@
       <c r="C24" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="21" t="s">
-        <v>111</v>
+      <c r="D24" s="46" t="s">
+        <v>107</v>
       </c>
       <c r="E24" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>113</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="F24" s="26"/>
       <c r="G24" s="32"/>
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
-      <c r="J24" s="31"/>
+      <c r="J24" s="34"/>
       <c r="K24" s="38"/>
       <c r="L24" s="39"/>
       <c r="M24" s="42"/>
@@ -2690,56 +2694,28 @@
       <c r="C25" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D25" s="21" t="s">
-        <v>111</v>
+      <c r="D25" s="46" t="s">
+        <v>107</v>
       </c>
       <c r="E25" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="G25" s="29" t="s">
-        <v>199</v>
-      </c>
-      <c r="H25" s="51">
-        <v>17</v>
-      </c>
-      <c r="I25" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J25" s="31" t="s">
-        <v>187</v>
-      </c>
-      <c r="K25" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="L25" s="39" t="s">
-        <v>32</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="F25" s="26"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="39"/>
       <c r="M25" s="42"/>
-      <c r="N25" s="42" t="s">
-        <v>216</v>
-      </c>
+      <c r="N25" s="42"/>
       <c r="O25" s="41"/>
-      <c r="P25" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>6</v>
-      </c>
-      <c r="R25" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="S25" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="T25" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="U25" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="P25" s="40"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="2"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
@@ -2751,26 +2727,24 @@
       <c r="C26" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D26" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="E26" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F26" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="G26" s="29" t="s">
-        <v>172</v>
+      <c r="D26" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="26"/>
+      <c r="G26" s="32" t="s">
+        <v>141</v>
       </c>
       <c r="H26" s="33">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I26" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="31" t="s">
-        <v>171</v>
+      <c r="J26" s="34" t="s">
+        <v>143</v>
       </c>
       <c r="K26" s="38" t="s">
         <v>69</v>
@@ -2780,62 +2754,84 @@
       </c>
       <c r="M26" s="42"/>
       <c r="N26" s="42" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="O26" s="41"/>
       <c r="P26" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q26" s="1">
         <v>6</v>
       </c>
       <c r="R26" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="S26" s="11" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="T26" s="11" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="U26" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="E27" s="45" t="s">
-        <v>112</v>
-      </c>
-      <c r="F27" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="G27" s="32"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="41"/>
-      <c r="P27" s="40"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
-      <c r="U27" s="2"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="60" t="s">
+        <v>217</v>
+      </c>
+      <c r="H27" s="50">
+        <v>17</v>
+      </c>
+      <c r="I27" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="73" t="s">
+        <v>218</v>
+      </c>
+      <c r="K27" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="L27" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="M27" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="N27" s="65"/>
+      <c r="O27" s="66"/>
+      <c r="P27" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q27" s="68">
+        <v>6</v>
+      </c>
+      <c r="R27" s="69" t="s">
+        <v>124</v>
+      </c>
+      <c r="S27" s="69" t="s">
+        <v>125</v>
+      </c>
+      <c r="T27" s="69" t="s">
+        <v>209</v>
+      </c>
+      <c r="U27" s="70" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
@@ -2854,49 +2850,23 @@
         <v>112</v>
       </c>
       <c r="F28" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="G28" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="H28" s="52">
-        <v>19</v>
-      </c>
-      <c r="I28" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="J28" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="K28" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="L28" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="M28" s="42" t="s">
-        <v>36</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="G28" s="32"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="31"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="42"/>
       <c r="N28" s="42"/>
       <c r="O28" s="41"/>
-      <c r="P28" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q28" s="1">
-        <v>6</v>
-      </c>
-      <c r="R28" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="S28" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="T28" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="U28" s="2" t="s">
-        <v>129</v>
-      </c>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="2"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
@@ -2911,27 +2881,53 @@
       <c r="D29" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="E29" s="25" t="s">
-        <v>117</v>
+      <c r="E29" s="45" t="s">
+        <v>112</v>
       </c>
       <c r="F29" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="G29" s="32"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="39"/>
+        <v>114</v>
+      </c>
+      <c r="G29" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="H29" s="33">
+        <v>18</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="K29" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="L29" s="39" t="s">
+        <v>32</v>
+      </c>
       <c r="M29" s="42"/>
-      <c r="N29" s="42"/>
+      <c r="N29" s="42" t="s">
+        <v>211</v>
+      </c>
       <c r="O29" s="41"/>
-      <c r="P29" s="40"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="11"/>
-      <c r="S29" s="11"/>
-      <c r="T29" s="11"/>
-      <c r="U29" s="2"/>
+      <c r="P29" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>6</v>
+      </c>
+      <c r="R29" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="S29" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="T29" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="U29" s="2" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
@@ -2946,23 +2942,23 @@
       <c r="D30" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="E30" s="25" t="s">
-        <v>117</v>
+      <c r="E30" s="45" t="s">
+        <v>112</v>
       </c>
       <c r="F30" s="26" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="H30" s="51">
-        <v>20</v>
+        <v>167</v>
+      </c>
+      <c r="H30" s="33">
+        <v>19</v>
       </c>
       <c r="I30" s="33" t="s">
         <v>20</v>
       </c>
       <c r="J30" s="31" t="s">
-        <v>201</v>
+        <v>166</v>
       </c>
       <c r="K30" s="38" t="s">
         <v>69</v>
@@ -2972,26 +2968,26 @@
       </c>
       <c r="M30" s="42"/>
       <c r="N30" s="42" t="s">
-        <v>216</v>
+        <v>47</v>
       </c>
       <c r="O30" s="41"/>
       <c r="P30" s="40" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q30" s="1">
         <v>6</v>
       </c>
       <c r="R30" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="S30" s="11" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="T30" s="11" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="U30" s="2" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
@@ -3007,53 +3003,27 @@
       <c r="D31" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="E31" s="25" t="s">
-        <v>117</v>
+      <c r="E31" s="45" t="s">
+        <v>112</v>
       </c>
       <c r="F31" s="26" t="s">
-        <v>120</v>
-      </c>
-      <c r="G31" s="32" t="s">
-        <v>137</v>
-      </c>
-      <c r="H31" s="51">
-        <v>21</v>
-      </c>
-      <c r="I31" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="K31" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="L31" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="M31" s="42" t="s">
-        <v>38</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="G31" s="32"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="42"/>
       <c r="N31" s="42"/>
       <c r="O31" s="41"/>
-      <c r="P31" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q31" s="1">
-        <v>6</v>
-      </c>
-      <c r="R31" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="S31" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="T31" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="U31" s="2" t="s">
-        <v>129</v>
-      </c>
+      <c r="P31" s="40"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="2"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
@@ -3068,32 +3038,34 @@
       <c r="D32" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="E32" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="F32" s="26"/>
+      <c r="E32" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="F32" s="26" t="s">
+        <v>116</v>
+      </c>
       <c r="G32" s="32" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="H32" s="33">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I32" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J32" s="34" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="K32" s="38" t="s">
         <v>69</v>
       </c>
       <c r="L32" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="M32" s="42"/>
-      <c r="N32" s="42" t="s">
-        <v>62</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="M32" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="N32" s="42"/>
       <c r="O32" s="41"/>
       <c r="P32" s="40" t="s">
         <v>19</v>
@@ -3102,19 +3074,19 @@
         <v>6</v>
       </c>
       <c r="R32" s="11" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="S32" s="11" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="T32" s="11" t="s">
-        <v>157</v>
+        <v>206</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>67</v>
       </c>
@@ -3125,51 +3097,29 @@
         <v>91</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E33" s="25"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="47" t="s">
-        <v>160</v>
-      </c>
-      <c r="H33" s="33">
-        <v>23</v>
-      </c>
-      <c r="I33" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="J33" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="K33" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="L33" s="39" t="s">
-        <v>32</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E33" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="G33" s="32"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="39"/>
       <c r="M33" s="42"/>
-      <c r="N33" s="42" t="s">
-        <v>64</v>
-      </c>
+      <c r="N33" s="42"/>
       <c r="O33" s="41"/>
-      <c r="P33" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q33" s="1">
-        <v>6</v>
-      </c>
-      <c r="R33" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="S33" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="T33" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="U33" s="2" t="s">
-        <v>154</v>
-      </c>
+      <c r="P33" s="40"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+      <c r="U33" s="2"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
@@ -3182,21 +3132,25 @@
         <v>91</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E34" s="25"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="32" t="s">
-        <v>159</v>
+        <v>111</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F34" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>195</v>
       </c>
       <c r="H34" s="33">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I34" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="J34" s="34" t="s">
-        <v>168</v>
+      <c r="J34" s="31" t="s">
+        <v>196</v>
       </c>
       <c r="K34" s="38" t="s">
         <v>69</v>
@@ -3206,7 +3160,7 @@
       </c>
       <c r="M34" s="42"/>
       <c r="N34" s="42" t="s">
-        <v>64</v>
+        <v>211</v>
       </c>
       <c r="O34" s="41"/>
       <c r="P34" s="40" t="s">
@@ -3216,130 +3170,138 @@
         <v>6</v>
       </c>
       <c r="R34" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="S34" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="T34" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="U34" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="S34" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="T34" s="11" t="s">
-        <v>162</v>
-      </c>
-      <c r="U34" s="2" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="35" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="17" t="s">
+      <c r="C35" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E35" s="25"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="47" t="s">
-        <v>174</v>
-      </c>
-      <c r="H35" s="33">
-        <v>25</v>
-      </c>
-      <c r="I35" s="33" t="s">
+      <c r="D35" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="E35" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="F35" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="G35" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="H35" s="50">
+        <v>22</v>
+      </c>
+      <c r="I35" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="J35" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="K35" s="38" t="s">
+      <c r="J35" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="K35" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="L35" s="39" t="s">
+      <c r="L35" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="M35" s="42"/>
-      <c r="N35" s="42" t="s">
+      <c r="M35" s="65"/>
+      <c r="N35" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="O35" s="41"/>
-      <c r="P35" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q35" s="1">
+      <c r="O35" s="66"/>
+      <c r="P35" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q35" s="68">
         <v>6</v>
       </c>
-      <c r="R35" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="S35" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="T35" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="U35" s="2" t="s">
-        <v>154</v>
+      <c r="R35" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="S35" s="69" t="s">
+        <v>147</v>
+      </c>
+      <c r="T35" s="69" t="s">
+        <v>178</v>
+      </c>
+      <c r="U35" s="70" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="57" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="58" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="47" t="s">
-        <v>175</v>
-      </c>
-      <c r="H36" s="33">
-        <v>26</v>
-      </c>
-      <c r="I36" s="33" t="s">
+      <c r="D36" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="E36" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="G36" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="H36" s="50">
+        <v>23</v>
+      </c>
+      <c r="I36" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="J36" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="K36" s="38" t="s">
+      <c r="J36" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="K36" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="L36" s="39" t="s">
+      <c r="L36" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="M36" s="42"/>
-      <c r="N36" s="42" t="s">
+      <c r="M36" s="65"/>
+      <c r="N36" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="O36" s="41"/>
-      <c r="P36" s="40" t="s">
+      <c r="O36" s="66"/>
+      <c r="P36" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="Q36" s="1">
+      <c r="Q36" s="68">
         <v>6</v>
       </c>
-      <c r="R36" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="S36" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="T36" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="U36" s="2" t="s">
-        <v>154</v>
+      <c r="R36" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="S36" s="69" t="s">
+        <v>147</v>
+      </c>
+      <c r="T36" s="69" t="s">
+        <v>171</v>
+      </c>
+      <c r="U36" s="70" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -3353,37 +3315,53 @@
         <v>91</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="E37" s="25"/>
+        <v>111</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>96</v>
+      </c>
       <c r="F37" s="26"/>
       <c r="G37" s="32" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="H37" s="33">
-        <v>27</v>
-      </c>
-      <c r="I37" s="33"/>
+        <v>24</v>
+      </c>
+      <c r="I37" s="33" t="s">
+        <v>20</v>
+      </c>
       <c r="J37" s="34" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="K37" s="38" t="s">
         <v>69</v>
       </c>
       <c r="L37" s="39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M37" s="42"/>
-      <c r="N37" s="42"/>
+      <c r="N37" s="42" t="s">
+        <v>62</v>
+      </c>
       <c r="O37" s="41"/>
       <c r="P37" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="11"/>
-      <c r="S37" s="11"/>
-      <c r="T37" s="11"/>
-      <c r="U37" s="2"/>
+      <c r="Q37" s="1">
+        <v>6</v>
+      </c>
+      <c r="R37" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="S37" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="T37" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="U37" s="2" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="38" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
@@ -3396,21 +3374,21 @@
         <v>91</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E38" s="25"/>
       <c r="F38" s="26"/>
-      <c r="G38" s="32" t="s">
-        <v>151</v>
+      <c r="G38" s="47" t="s">
+        <v>155</v>
       </c>
       <c r="H38" s="33">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I38" s="33" t="s">
         <v>20</v>
       </c>
       <c r="J38" s="34" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="K38" s="38" t="s">
         <v>69</v>
@@ -3420,7 +3398,7 @@
       </c>
       <c r="M38" s="42"/>
       <c r="N38" s="42" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="O38" s="41"/>
       <c r="P38" s="40" t="s">
@@ -3430,19 +3408,19 @@
         <v>6</v>
       </c>
       <c r="R38" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="S38" s="11" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="T38" s="11" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="U38" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>67</v>
       </c>
@@ -3452,20 +3430,22 @@
       <c r="C39" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="D39" s="21"/>
+      <c r="D39" s="21" t="s">
+        <v>121</v>
+      </c>
       <c r="E39" s="25"/>
       <c r="F39" s="26"/>
-      <c r="G39" s="47" t="s">
-        <v>204</v>
+      <c r="G39" s="32" t="s">
+        <v>154</v>
       </c>
       <c r="H39" s="33">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I39" s="33" t="s">
         <v>20</v>
       </c>
       <c r="J39" s="34" t="s">
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="K39" s="38" t="s">
         <v>69</v>
@@ -3475,96 +3455,182 @@
       </c>
       <c r="M39" s="42"/>
       <c r="N39" s="42" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O39" s="41"/>
       <c r="P39" s="40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q39" s="1">
         <v>6</v>
       </c>
       <c r="R39" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="S39" s="11" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="T39" s="11" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="U39" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="19"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="21"/>
+      <c r="A40" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="21" t="s">
+        <v>122</v>
+      </c>
       <c r="E40" s="25"/>
       <c r="F40" s="26"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="33"/>
+      <c r="G40" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="H40" s="33">
+        <v>27</v>
+      </c>
       <c r="I40" s="33"/>
-      <c r="J40" s="34"/>
-      <c r="K40" s="38"/>
-      <c r="L40" s="39"/>
+      <c r="J40" s="34" t="s">
+        <v>177</v>
+      </c>
+      <c r="K40" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="L40" s="39" t="s">
+        <v>33</v>
+      </c>
       <c r="M40" s="42"/>
       <c r="N40" s="42"/>
       <c r="O40" s="41"/>
-      <c r="P40" s="40"/>
+      <c r="P40" s="40" t="s">
+        <v>19</v>
+      </c>
       <c r="Q40" s="1"/>
       <c r="R40" s="11"/>
       <c r="S40" s="11"/>
       <c r="T40" s="11"/>
       <c r="U40" s="2"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
-      <c r="B41" s="19"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="21"/>
+    <row r="41" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>122</v>
+      </c>
       <c r="E41" s="25"/>
       <c r="F41" s="26"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="33"/>
-      <c r="J41" s="34"/>
-      <c r="K41" s="38"/>
-      <c r="L41" s="39"/>
+      <c r="G41" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="H41" s="33">
+        <v>28</v>
+      </c>
+      <c r="I41" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J41" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="K41" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="L41" s="39" t="s">
+        <v>32</v>
+      </c>
       <c r="M41" s="42"/>
-      <c r="N41" s="42"/>
+      <c r="N41" s="42" t="s">
+        <v>81</v>
+      </c>
       <c r="O41" s="41"/>
-      <c r="P41" s="40"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="11"/>
-      <c r="S41" s="11"/>
-      <c r="T41" s="11"/>
-      <c r="U41" s="2"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-      <c r="B42" s="19"/>
-      <c r="C42" s="20"/>
+      <c r="P41" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>6</v>
+      </c>
+      <c r="R41" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="S41" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="T41" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="U41" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>91</v>
+      </c>
       <c r="D42" s="21"/>
       <c r="E42" s="25"/>
       <c r="F42" s="26"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="33"/>
-      <c r="J42" s="31"/>
-      <c r="K42" s="38"/>
-      <c r="L42" s="39"/>
+      <c r="G42" s="47" t="s">
+        <v>199</v>
+      </c>
+      <c r="H42" s="33">
+        <v>29</v>
+      </c>
+      <c r="I42" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="J42" s="34" t="s">
+        <v>198</v>
+      </c>
+      <c r="K42" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="L42" s="39" t="s">
+        <v>32</v>
+      </c>
       <c r="M42" s="42"/>
-      <c r="N42" s="42"/>
+      <c r="N42" s="42" t="s">
+        <v>63</v>
+      </c>
       <c r="O42" s="41"/>
-      <c r="P42" s="40"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="11"/>
-      <c r="S42" s="11"/>
-      <c r="T42" s="11"/>
-      <c r="U42" s="2"/>
+      <c r="P42" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>6</v>
+      </c>
+      <c r="R42" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="S42" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="T42" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="U42" s="2" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="18"/>
@@ -3612,7 +3678,7 @@
       <c r="T44" s="11"/>
       <c r="U44" s="2"/>
     </row>
-    <row r="45" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="19"/>
       <c r="C45" s="20"/>
@@ -3622,7 +3688,7 @@
       <c r="G45" s="32"/>
       <c r="H45" s="33"/>
       <c r="I45" s="33"/>
-      <c r="J45" s="34"/>
+      <c r="J45" s="31"/>
       <c r="K45" s="38"/>
       <c r="L45" s="39"/>
       <c r="M45" s="42"/>
@@ -3681,7 +3747,7 @@
       <c r="T47" s="11"/>
       <c r="U47" s="2"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
       <c r="B48" s="19"/>
       <c r="C48" s="20"/>
@@ -3777,9 +3843,9 @@
       <c r="A52" s="18"/>
       <c r="B52" s="19"/>
       <c r="C52" s="20"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="28"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="26"/>
       <c r="G52" s="32"/>
       <c r="H52" s="33"/>
       <c r="I52" s="33"/>
@@ -3800,9 +3866,9 @@
       <c r="A53" s="18"/>
       <c r="B53" s="19"/>
       <c r="C53" s="20"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="28"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="26"/>
       <c r="G53" s="32"/>
       <c r="H53" s="33"/>
       <c r="I53" s="33"/>
@@ -3823,9 +3889,9 @@
       <c r="A54" s="18"/>
       <c r="B54" s="19"/>
       <c r="C54" s="20"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="28"/>
+      <c r="D54" s="21"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="26"/>
       <c r="G54" s="32"/>
       <c r="H54" s="33"/>
       <c r="I54" s="33"/>
@@ -4831,8 +4897,82 @@
       <c r="T97" s="11"/>
       <c r="U97" s="2"/>
     </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A98" s="18"/>
+      <c r="B98" s="19"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="28"/>
+      <c r="G98" s="32"/>
+      <c r="H98" s="33"/>
+      <c r="I98" s="33"/>
+      <c r="J98" s="34"/>
+      <c r="K98" s="38"/>
+      <c r="L98" s="39"/>
+      <c r="M98" s="42"/>
+      <c r="N98" s="42"/>
+      <c r="O98" s="41"/>
+      <c r="P98" s="40"/>
+      <c r="Q98" s="1"/>
+      <c r="R98" s="11"/>
+      <c r="S98" s="11"/>
+      <c r="T98" s="11"/>
+      <c r="U98" s="2"/>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A99" s="18"/>
+      <c r="B99" s="19"/>
+      <c r="C99" s="20"/>
+      <c r="D99" s="22"/>
+      <c r="E99" s="27"/>
+      <c r="F99" s="28"/>
+      <c r="G99" s="32"/>
+      <c r="H99" s="33"/>
+      <c r="I99" s="33"/>
+      <c r="J99" s="34"/>
+      <c r="K99" s="38"/>
+      <c r="L99" s="39"/>
+      <c r="M99" s="42"/>
+      <c r="N99" s="42"/>
+      <c r="O99" s="41"/>
+      <c r="P99" s="40"/>
+      <c r="Q99" s="1"/>
+      <c r="R99" s="11"/>
+      <c r="S99" s="11"/>
+      <c r="T99" s="11"/>
+      <c r="U99" s="2"/>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A100" s="18"/>
+      <c r="B100" s="19"/>
+      <c r="C100" s="20"/>
+      <c r="D100" s="22"/>
+      <c r="E100" s="27"/>
+      <c r="F100" s="28"/>
+      <c r="G100" s="32"/>
+      <c r="H100" s="33"/>
+      <c r="I100" s="33"/>
+      <c r="J100" s="34"/>
+      <c r="K100" s="38"/>
+      <c r="L100" s="39"/>
+      <c r="M100" s="42"/>
+      <c r="N100" s="42"/>
+      <c r="O100" s="41"/>
+      <c r="P100" s="40"/>
+      <c r="Q100" s="1"/>
+      <c r="R100" s="11"/>
+      <c r="S100" s="11"/>
+      <c r="T100" s="11"/>
+      <c r="U100" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="U1:U2"/>
@@ -4847,11 +4987,6 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>